<commit_message>
Added size with analytical se
</commit_message>
<xml_diff>
--- a/Case assignment - Results.xlsx
+++ b/Case assignment - Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">rho</t>
   </si>
@@ -37,7 +37,10 @@
     <t xml:space="preserve">result_an</t>
   </si>
   <si>
-    <t xml:space="preserve">size</t>
+    <t xml:space="preserve">size_an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size_ese</t>
   </si>
   <si>
     <t xml:space="preserve">asymptotic_assumption</t>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
   </si>
 </sst>
 </file>
@@ -415,6 +421,9 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -436,20 +445,23 @@
         <v>0.176047191503766</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.158113883008419</v>
       </c>
       <c r="H2" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.18</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.15625</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.25</v>
       </c>
       <c r="K2" t="n">
         <v>-0.25</v>
       </c>
+      <c r="L2" t="n">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -471,20 +483,23 @@
         <v>0.0630455150640945</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
         <v>1.5625</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-0.25</v>
       </c>
       <c r="K3" t="n">
         <v>-0.25</v>
       </c>
+      <c r="L3" t="n">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -506,20 +521,23 @@
         <v>0.115063398861566</v>
       </c>
       <c r="G4" t="n">
-        <v>0.316227766016838</v>
+        <v>0.1</v>
       </c>
       <c r="H4" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.13</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.01</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-0.1</v>
       </c>
       <c r="K4" t="n">
         <v>-0.1</v>
       </c>
+      <c r="L4" t="n">
+        <v>-0.1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -541,20 +559,23 @@
         <v>0.0374738211652785</v>
       </c>
       <c r="G5" t="n">
-        <v>0.316227766016838</v>
+        <v>0.0316227766016838</v>
       </c>
       <c r="H5" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.79</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-0.1</v>
       </c>
       <c r="K5" t="n">
         <v>-0.1</v>
       </c>
+      <c r="L5" t="n">
+        <v>-0.1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -576,20 +597,23 @@
         <v>0.0741323114165449</v>
       </c>
       <c r="G6" t="n">
-        <v>0.223606797749979</v>
+        <v>0.0707106781186548</v>
       </c>
       <c r="H6" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.13</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.00125</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-0.05</v>
       </c>
       <c r="K6" t="n">
         <v>-0.05</v>
       </c>
+      <c r="L6" t="n">
+        <v>-0.05</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -611,20 +635,23 @@
         <v>0.0240055107309665</v>
       </c>
       <c r="G7" t="n">
-        <v>0.223606797749979</v>
+        <v>0.0223606797749979</v>
       </c>
       <c r="H7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.71</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.0125</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-0.05</v>
       </c>
       <c r="K7" t="n">
         <v>-0.05</v>
       </c>
+      <c r="L7" t="n">
+        <v>-0.05</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -646,20 +673,23 @@
         <v>0.0470884092195551</v>
       </c>
       <c r="G8" t="n">
-        <v>0.14142135623731</v>
+        <v>0.0447213595499958</v>
       </c>
       <c r="H8" t="n">
         <v>0.07</v>
       </c>
       <c r="I8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J8" t="n">
         <v>0.00008</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-0.02</v>
       </c>
       <c r="K8" t="n">
         <v>-0.02</v>
       </c>
+      <c r="L8" t="n">
+        <v>-0.02</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -681,18 +711,21 @@
         <v>0.0153535407030825</v>
       </c>
       <c r="G9" t="n">
-        <v>0.14142135623731</v>
+        <v>0.014142135623731</v>
       </c>
       <c r="H9" t="n">
         <v>0.36</v>
       </c>
       <c r="I9" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="J9" t="n">
         <v>0.0008</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>-0.02</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>-0.02</v>
       </c>
     </row>
@@ -716,18 +749,21 @@
         <v>0.215113007650877</v>
       </c>
       <c r="G10" t="n">
-        <v>0.577350269189626</v>
+        <v>0.182574185835055</v>
       </c>
       <c r="H10" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.49</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.15625</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>-0.375</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.125</v>
       </c>
     </row>
@@ -751,18 +787,21 @@
         <v>0.0781748073553783</v>
       </c>
       <c r="G11" t="n">
-        <v>0.577350269189626</v>
+        <v>0.0577350269189626</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
         <v>1.5625</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>-0.375</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.125</v>
       </c>
     </row>
@@ -786,18 +825,21 @@
         <v>0.112033438370566</v>
       </c>
       <c r="G12" t="n">
-        <v>0.365148371670111</v>
+        <v>0.115470053837925</v>
       </c>
       <c r="H12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.41</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.01</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>-0.15</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -821,18 +863,21 @@
         <v>0.0362222990641808</v>
       </c>
       <c r="G13" t="n">
-        <v>0.365148371670111</v>
+        <v>0.0365148371670111</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
         <v>0.1</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>-0.15</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -856,18 +901,21 @@
         <v>0.0665886050554622</v>
       </c>
       <c r="G14" t="n">
-        <v>0.258198889747161</v>
+        <v>0.0816496580927726</v>
       </c>
       <c r="H14" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.25</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.00125</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>-0.075</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.425</v>
       </c>
     </row>
@@ -891,18 +939,21 @@
         <v>0.0203017240647192</v>
       </c>
       <c r="G15" t="n">
-        <v>0.258198889747161</v>
+        <v>0.0258198889747161</v>
       </c>
       <c r="H15" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.98</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.0125</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>-0.075</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0.425</v>
       </c>
     </row>
@@ -926,18 +977,21 @@
         <v>0.0410547933937812</v>
       </c>
       <c r="G16" t="n">
-        <v>0.163299316185545</v>
+        <v>0.0516397779494322</v>
       </c>
       <c r="H16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.13</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.00008</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>-0.03</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.47</v>
       </c>
     </row>
@@ -961,18 +1015,21 @@
         <v>0.0122893400468812</v>
       </c>
       <c r="G17" t="n">
-        <v>0.163299316185545</v>
+        <v>0.0163299316185545</v>
       </c>
       <c r="H17" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.71</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.0008</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>-0.03</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.47</v>
       </c>
     </row>
@@ -996,18 +1053,21 @@
         <v>0.220089142637865</v>
       </c>
       <c r="G18" t="n">
-        <v>1.14707866935281</v>
+        <v>0.362738125055006</v>
       </c>
       <c r="H18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.05</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.15625</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>-0.475</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>0.425</v>
       </c>
     </row>
@@ -1031,18 +1091,21 @@
         <v>0.065011479172854</v>
       </c>
       <c r="G19" t="n">
-        <v>1.14707866935281</v>
+        <v>0.114707866935281</v>
       </c>
       <c r="H19" t="n">
         <v>1</v>
       </c>
       <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
         <v>1.5625</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>-0.475</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>0.425</v>
       </c>
     </row>
@@ -1066,18 +1129,21 @@
         <v>0.0972119931703986</v>
       </c>
       <c r="G20" t="n">
-        <v>0.725476250110012</v>
+        <v>0.229415733870562</v>
       </c>
       <c r="H20" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I20" t="n">
         <v>0.85</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.01</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>-0.19</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -1101,18 +1167,21 @@
         <v>0.0296614074330449</v>
       </c>
       <c r="G21" t="n">
-        <v>0.725476250110012</v>
+        <v>0.0725476250110012</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
       </c>
       <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
         <v>0.1</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>-0.19</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -1136,18 +1205,21 @@
         <v>0.0547121946409047</v>
       </c>
       <c r="G22" t="n">
-        <v>0.512989176042577</v>
+        <v>0.162221421130763</v>
       </c>
       <c r="H22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I22" t="n">
         <v>0.78</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.00125</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>-0.095</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>0.805</v>
       </c>
     </row>
@@ -1171,18 +1243,21 @@
         <v>0.0181104914066377</v>
       </c>
       <c r="G23" t="n">
-        <v>0.512989176042577</v>
+        <v>0.0512989176042577</v>
       </c>
       <c r="H23" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="I23" t="n">
         <v>1</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.0125</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>-0.095</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>0.805</v>
       </c>
     </row>
@@ -1206,18 +1281,21 @@
         <v>0.0283864724504793</v>
       </c>
       <c r="G24" t="n">
-        <v>0.324442842261525</v>
+        <v>0.102597835208515</v>
       </c>
       <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.54</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.00008</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>-0.038</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>0.862</v>
       </c>
     </row>
@@ -1241,18 +1319,21 @@
         <v>0.00782001446690646</v>
       </c>
       <c r="G25" t="n">
-        <v>0.324442842261525</v>
+        <v>0.0324442842261525</v>
       </c>
       <c r="H25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I25" t="n">
         <v>1</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>0.0008</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>-0.038</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>0.862</v>
       </c>
     </row>
@@ -1281,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1290,7 +1371,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
@@ -1870,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1879,7 +1960,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">

</xml_diff>